<commit_message>
completed the preliminary terrain system, including the definition of terrain, the definition of events
</commit_message>
<xml_diff>
--- a/Assets/_Excel/enemy.xlsx
+++ b/Assets/_Excel/enemy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\UnityDemo\BattleFlagGame\Assets\_Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unity\BattleFlagGameStudy\Assets\_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC47753-B4BF-4393-8AD1-A112E8DF09A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3380D398-249E-4CFE-BD3D-A88C0A6D63C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6960" yWindow="1290" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -113,7 +113,6 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -459,13 +458,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +490,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +516,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>10001</v>
       </c>
@@ -543,7 +542,7 @@
         <v>10003</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>10002</v>
       </c>
@@ -569,7 +568,7 @@
         <v>10004</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>10003</v>
       </c>

</xml_diff>

<commit_message>
only fixed some bug
</commit_message>
<xml_diff>
--- a/Assets/_Excel/enemy.xlsx
+++ b/Assets/_Excel/enemy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unity\BattleFlagGameStudy\Assets\_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3380D398-249E-4CFE-BD3D-A88C0A6D63C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85BDC21-EEC8-4641-81B2-74315361E808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="1290" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2865" windowWidth="27675" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Id</t>
   </si>
@@ -95,6 +95,14 @@
   </si>
   <si>
     <t>enemy03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交互</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -144,12 +152,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -456,15 +467,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:H5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,8 +500,11 @@
       <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="I1" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,8 +529,11 @@
       <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="I2" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>10001</v>
       </c>
@@ -541,8 +558,11 @@
       <c r="H3" s="1">
         <v>10003</v>
       </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>10002</v>
       </c>
@@ -567,8 +587,11 @@
       <c r="H4" s="2">
         <v>10004</v>
       </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>10003</v>
       </c>
@@ -592,6 +615,9 @@
       </c>
       <c r="H5" s="1">
         <v>10005</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>